<commit_message>
Plant and non plant analysis
</commit_message>
<xml_diff>
--- a/Varroa 2/Varroa_genus.xlsx
+++ b/Varroa 2/Varroa_genus.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\honeyDSM-seq\Varroa 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sol/Documents/GitHub/Direct-shotgun-metagenomics-pub/Varroa 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CB4F8B2-6335-4737-A16C-591DD69F6BA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D78A90-6F5A-F14E-968A-5DDC0742A2D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{B08D222D-720C-7C4C-92C0-0703F2971EE5}"/>
+    <workbookView xWindow="1840" yWindow="460" windowWidth="25260" windowHeight="16220" activeTab="1" xr2:uid="{B08D222D-720C-7C4C-92C0-0703F2971EE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Varroa 2" sheetId="3" r:id="rId1"/>
-    <sheet name="export from apiary" sheetId="2" r:id="rId2"/>
+    <sheet name="Final" sheetId="4" r:id="rId2"/>
+    <sheet name="export from apiary" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="35">
   <si>
     <t>hive</t>
   </si>
@@ -119,6 +120,18 @@
   </si>
   <si>
     <t>DeSeq2_SM</t>
+  </si>
+  <si>
+    <t>Monitoring</t>
+  </si>
+  <si>
+    <t>Natural_Fall</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Reads</t>
   </si>
 </sst>
 </file>
@@ -154,7 +167,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -183,9 +195,9 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -503,13 +515,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C001B4C-6C4E-734C-BD48-CBB43D45280A}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,37 +563,37 @@
       </c>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>3282782</v>
       </c>
       <c r="C2">
         <v>874</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <f>C2*(1/B2)*1000000</f>
         <v>266.2375996944055</v>
       </c>
       <c r="E2">
         <v>34</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>4058520</v>
       </c>
       <c r="G2">
         <v>1000</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <f t="shared" ref="H2:H5" si="0">G2*(1/F2)*1000000</f>
         <v>246.39523767284624</v>
       </c>
       <c r="I2">
         <v>63</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="4">
         <v>5.8</v>
       </c>
       <c r="K2">
@@ -594,37 +606,37 @@
         <v>70.774074074074136</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>1444924</v>
       </c>
       <c r="C3">
         <v>977</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <f t="shared" ref="D3:D5" si="1">C3*(1/B3)*1000000</f>
         <v>676.16013022138179</v>
       </c>
       <c r="E3">
         <v>59</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>8160732</v>
       </c>
       <c r="G3">
         <v>772</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <f>G3*(1/F3)*1000000</f>
         <v>94.59935701846355</v>
       </c>
       <c r="I3">
         <v>30</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>30</v>
       </c>
       <c r="K3">
@@ -634,40 +646,40 @@
         <v>28.125</v>
       </c>
       <c r="M3">
-        <v>20.083333333333332</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>41.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>2379244</v>
       </c>
       <c r="C4">
         <v>2309</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <f t="shared" si="1"/>
         <v>970.47633618073644</v>
       </c>
       <c r="E4">
         <v>52</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>3619844</v>
       </c>
       <c r="G4">
         <v>1122</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <f t="shared" si="0"/>
         <v>309.9581086919768</v>
       </c>
       <c r="I4">
         <v>69</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>13.047619047619051</v>
       </c>
       <c r="K4">
@@ -680,37 +692,37 @@
         <v>31.151785714285715</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>2280627</v>
       </c>
       <c r="C5">
         <v>2196</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <f t="shared" si="1"/>
         <v>962.8930991345801</v>
       </c>
       <c r="E5">
         <v>52</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>2038989</v>
       </c>
       <c r="G5">
         <v>1128</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f t="shared" si="0"/>
         <v>553.21534348640432</v>
       </c>
       <c r="I5">
         <v>22</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>3</v>
       </c>
       <c r="K5">
@@ -729,16 +741,1139 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B91DFE-BB5F-4E4E-8F8F-C92C36D9663D}">
+  <dimension ref="A1:E65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="22.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>266.2375996944055</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>266.2375996944055</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>9.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>266.2375996944055</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>16.259999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>266.2375996944055</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>70.774074074074136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>676.16013022138179</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>676.16013022138179</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>28.125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>676.16013022138179</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>28.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>676.16013022138179</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>41.8611111111111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>970.47633618073644</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>13.047619047619051</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>970.47633618073644</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>13.047619047619051</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>970.47633618073644</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>22.776190476190482</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>970.47633618073644</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13">
+        <v>31.151785714285715</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>962.8930991345801</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>962.8930991345801</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>962.8930991345801</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <v>14.666666666666671</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>962.8930991345801</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17">
+        <v>15.489583333333337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19">
+        <v>9.15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <v>16.259999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21">
+        <v>70.774074074074136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23">
+        <v>28.125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24">
+        <v>28.125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25">
+        <v>41.8611111111111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>52</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26">
+        <v>13.047619047619051</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>52</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27">
+        <v>13.047619047619051</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28">
+        <v>22.776190476190482</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29">
+        <v>31.151785714285715</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30">
+        <v>52</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31">
+        <v>52</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32">
+        <v>52</v>
+      </c>
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32">
+        <v>14.666666666666671</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33">
+        <v>52</v>
+      </c>
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33">
+        <v>15.489583333333337</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34">
+        <v>246.39523767284624</v>
+      </c>
+      <c r="D34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35">
+        <v>246.39523767284624</v>
+      </c>
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35">
+        <v>9.15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36">
+        <v>246.39523767284624</v>
+      </c>
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36">
+        <v>16.259999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37">
+        <v>246.39523767284624</v>
+      </c>
+      <c r="D37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37">
+        <v>70.774074074074136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38">
+        <v>94.59935701846355</v>
+      </c>
+      <c r="D38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39">
+        <v>94.59935701846355</v>
+      </c>
+      <c r="D39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39">
+        <v>28.125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40">
+        <v>94.59935701846355</v>
+      </c>
+      <c r="D40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40">
+        <v>28.125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41">
+        <v>94.59935701846355</v>
+      </c>
+      <c r="D41" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41">
+        <v>41.8611111111111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42">
+        <v>309.9581086919768</v>
+      </c>
+      <c r="D42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42">
+        <v>13.047619047619051</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43">
+        <v>309.9581086919768</v>
+      </c>
+      <c r="D43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43">
+        <v>13.047619047619051</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44">
+        <v>309.9581086919768</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44">
+        <v>22.776190476190482</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45">
+        <v>309.9581086919768</v>
+      </c>
+      <c r="D45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45">
+        <v>31.151785714285715</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46">
+        <v>553.21534348640432</v>
+      </c>
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47">
+        <v>553.21534348640432</v>
+      </c>
+      <c r="D47" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48">
+        <v>553.21534348640432</v>
+      </c>
+      <c r="D48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48">
+        <v>14.666666666666671</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49">
+        <v>553.21534348640432</v>
+      </c>
+      <c r="D49" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49">
+        <v>15.489583333333337</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50">
+        <v>63</v>
+      </c>
+      <c r="D50" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51">
+        <v>63</v>
+      </c>
+      <c r="D51" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51">
+        <v>9.15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52">
+        <v>63</v>
+      </c>
+      <c r="D52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52">
+        <v>16.259999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53">
+        <v>63</v>
+      </c>
+      <c r="D53" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53">
+        <v>70.774074074074136</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54">
+        <v>30</v>
+      </c>
+      <c r="D54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E54">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55">
+        <v>30</v>
+      </c>
+      <c r="D55" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55">
+        <v>28.125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56">
+        <v>30</v>
+      </c>
+      <c r="D56" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56">
+        <v>28.125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57">
+        <v>30</v>
+      </c>
+      <c r="D57" t="s">
+        <v>21</v>
+      </c>
+      <c r="E57">
+        <v>41.8611111111111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58">
+        <v>69</v>
+      </c>
+      <c r="D58" t="s">
+        <v>22</v>
+      </c>
+      <c r="E58">
+        <v>13.047619047619051</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s">
+        <v>30</v>
+      </c>
+      <c r="C59">
+        <v>69</v>
+      </c>
+      <c r="D59" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59">
+        <v>13.047619047619051</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60">
+        <v>69</v>
+      </c>
+      <c r="D60" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60">
+        <v>22.776190476190482</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61">
+        <v>69</v>
+      </c>
+      <c r="D61" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61">
+        <v>31.151785714285715</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62">
+        <v>22</v>
+      </c>
+      <c r="D62" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" t="s">
+        <v>30</v>
+      </c>
+      <c r="C63">
+        <v>22</v>
+      </c>
+      <c r="D63" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" t="s">
+        <v>30</v>
+      </c>
+      <c r="C64">
+        <v>22</v>
+      </c>
+      <c r="D64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E64">
+        <v>14.666666666666671</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65">
+        <v>22</v>
+      </c>
+      <c r="D65" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65">
+        <v>15.489583333333337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C3DD89-0D21-5342-972B-E1A667E0B403}">
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="H1" sqref="H1:M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -773,8 +1908,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
         <v>43808</v>
       </c>
       <c r="B2" t="s">
@@ -812,8 +1947,8 @@
         <v>70.774074074074136</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
         <v>43780</v>
       </c>
       <c r="B3" t="s">
@@ -848,11 +1983,11 @@
       </c>
       <c r="M3">
         <f>AVERAGE(E26:E28)</f>
-        <v>20.083333333333332</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+        <v>41.8611111111111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
         <v>43767</v>
       </c>
       <c r="B4" t="s">
@@ -890,8 +2025,8 @@
         <v>31.151785714285715</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
         <v>43760</v>
       </c>
       <c r="B5" t="s">
@@ -929,8 +2064,8 @@
         <v>15.489583333333337</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
         <v>43739</v>
       </c>
       <c r="B6" t="s">
@@ -946,8 +2081,8 @@
         <v>23.75</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
         <v>43731</v>
       </c>
       <c r="B7" t="s">
@@ -963,8 +2098,8 @@
         <v>28.25</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
         <v>43724</v>
       </c>
       <c r="B8" t="s">
@@ -980,8 +2115,8 @@
         <v>90.3333333333333</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
         <v>43717</v>
       </c>
       <c r="B9" t="s">
@@ -997,8 +2132,8 @@
         <v>186.666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
         <v>43710</v>
       </c>
       <c r="B10" t="s">
@@ -1014,8 +2149,8 @@
         <v>186.666666666667</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
         <v>43704</v>
       </c>
       <c r="B11" t="s">
@@ -1031,8 +2166,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <v>43697</v>
       </c>
       <c r="B12" t="s">
@@ -1048,8 +2183,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
         <v>43689</v>
       </c>
       <c r="B13" t="s">
@@ -1065,8 +2200,8 @@
         <v>111.333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
         <v>43682</v>
       </c>
       <c r="B14" t="s">
@@ -1082,8 +2217,8 @@
         <v>177.666666666667</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
         <v>43675</v>
       </c>
       <c r="B15" t="s">
@@ -1099,8 +2234,8 @@
         <v>83.6666666666667</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
         <v>43668</v>
       </c>
       <c r="B16" t="s">
@@ -1116,8 +2251,8 @@
         <v>0.66666666666666696</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
         <v>43662</v>
       </c>
       <c r="B17" t="s">
@@ -1133,8 +2268,8 @@
         <v>9.4285714285714306</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
         <v>43651</v>
       </c>
       <c r="B18" t="s">
@@ -1150,8 +2285,8 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
         <v>43644</v>
       </c>
       <c r="B19" t="s">
@@ -1167,8 +2302,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
         <v>43637</v>
       </c>
       <c r="B20" t="s">
@@ -1184,8 +2319,8 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
         <v>43630</v>
       </c>
       <c r="B21" t="s">
@@ -1201,8 +2336,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
         <v>43620</v>
       </c>
       <c r="B22" t="s">
@@ -1218,8 +2353,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
         <v>43605</v>
       </c>
       <c r="B23" t="s">
@@ -1235,8 +2370,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
         <v>43578</v>
       </c>
       <c r="B24" t="s">
@@ -1249,11 +2384,11 @@
         <v>13900</v>
       </c>
       <c r="E24">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
+        <v>880.33333333333303</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
         <v>43532</v>
       </c>
       <c r="B25" t="s">
@@ -1266,11 +2401,11 @@
         <v>7800</v>
       </c>
       <c r="E25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
         <v>43594</v>
       </c>
       <c r="B26" t="s">
@@ -1286,8 +2421,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
         <v>43578</v>
       </c>
       <c r="B27" t="s">
@@ -1303,8 +2438,8 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
         <v>43532</v>
       </c>
       <c r="B28" t="s">
@@ -1317,11 +2452,11 @@
         <v>5200</v>
       </c>
       <c r="E28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
+        <v>69.3333333333333</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
         <v>43668</v>
       </c>
       <c r="B29" t="s">
@@ -1337,8 +2472,8 @@
         <v>14.6666666666667</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
         <v>43662</v>
       </c>
       <c r="B30" t="s">
@@ -1354,8 +2489,8 @@
         <v>11.4285714285714</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
         <v>43637</v>
       </c>
       <c r="B31" t="s">
@@ -1371,8 +2506,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
         <v>43630</v>
       </c>
       <c r="B32" t="s">
@@ -1388,8 +2523,8 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
         <v>43620</v>
       </c>
       <c r="B33" t="s">
@@ -1405,8 +2540,8 @@
         <v>42.285714285714299</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
         <v>43605</v>
       </c>
       <c r="B34" t="s">
@@ -1422,8 +2557,8 @@
         <v>53.3333333333333</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
         <v>43594</v>
       </c>
       <c r="B35" t="s">
@@ -1439,8 +2574,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
         <v>43578</v>
       </c>
       <c r="B36" t="s">
@@ -1456,8 +2591,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
         <v>43532</v>
       </c>
       <c r="B37" t="s">
@@ -1470,11 +2605,11 @@
         <v>9100</v>
       </c>
       <c r="E37">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
+        <v>485.33333333333297</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
         <v>43651</v>
       </c>
       <c r="B38" t="s">
@@ -1490,8 +2625,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
         <v>43644</v>
       </c>
       <c r="B39" t="s">
@@ -1507,8 +2642,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="4">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="6">
         <v>43637</v>
       </c>
       <c r="B40" t="s">
@@ -1524,8 +2659,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="6">
         <v>43630</v>
       </c>
       <c r="B41" t="s">
@@ -1541,8 +2676,8 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="6">
         <v>43620</v>
       </c>
       <c r="B42" t="s">
@@ -1558,8 +2693,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="6">
         <v>43605</v>
       </c>
       <c r="B43" t="s">
@@ -1575,8 +2710,8 @@
         <v>26.6666666666667</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="6">
         <v>43594</v>
       </c>
       <c r="B44" t="s">
@@ -1592,8 +2727,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="6">
         <v>43573</v>
       </c>
       <c r="B45" t="s">
@@ -1609,8 +2744,8 @@
         <v>21.25</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="6">
         <v>43532</v>
       </c>
       <c r="B46" t="s">
@@ -1623,10 +2758,13 @@
         <v>7100</v>
       </c>
       <c r="E46">
-        <v>21</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E46">
+    <sortCondition ref="B1:B46"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>